<commit_message>
solucionado el problema para mostrar los equipos y fechas en el documento excel, reescritas las estructuras en formato de c++
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -14,132 +14,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
-  <si>
-    <t>��C_x0002_</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+  <si>
+    <t>Colo-Colo</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>0_x0008_D_x0002_</t>
-  </si>
-  <si>
-    <t>�_x0003_D_x0002_</t>
+    <t>Universidad de Chile</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>p_x0002_D_x0002_</t>
-  </si>
-  <si>
-    <t>�_x0005_D_x0002_</t>
+    <t>Universidad Catolica</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>p�C_x0002_</t>
-  </si>
-  <si>
-    <t>��C_x0002_</t>
+    <t>Union Española</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>��C_x0002_</t>
-  </si>
-  <si>
-    <t>��C_x0002_</t>
+    <t>Audax Italiano</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>(�C_x0002_</t>
+    <t>Curicó Unido</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t xml:space="preserve"> �C_x0002_</t>
+    <t>Deportes Antofagasta</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>@�C_x0002_</t>
-  </si>
-  <si>
-    <t>`�C_x0002_</t>
+    <t>Deportes Iquique</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>��C_x0002_</t>
+    <t>Deportes Temuco</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t xml:space="preserve"> �C_x0002_</t>
-  </si>
-  <si>
-    <t>H�C_x0002_</t>
+    <t>Everton</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>h�C_x0002_</t>
-  </si>
-  <si>
-    <t>��C_x0002_</t>
+    <t>Huachipato</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>��C_x0002_</t>
-  </si>
-  <si>
-    <t>��C_x0002_</t>
+    <t>O'Higgins</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>��C_x0002_</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> �C_x0002_</t>
+    <t>Palestino</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>@�C_x0002_</t>
-  </si>
-  <si>
-    <t>h�C_x0002_</t>
+    <t>San Luis</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>�_x0003_D_x0002_</t>
-  </si>
-  <si>
-    <t>_x0010__x0008_D_x0002_</t>
+    <t>Santiago Wanderers</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>_x0010_�C_x0002_</t>
+    <t>Universidad de Concepción</t>
   </si>
 </sst>
 </file>
@@ -499,147 +466,156 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>